<commit_message>
completed guides for vertuo coffee
</commit_message>
<xml_diff>
--- a/RawData.xlsx
+++ b/RawData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="730">
   <si>
     <t>ID</t>
   </si>
@@ -1131,13 +1131,1084 @@
   </si>
   <si>
     <t>Sweet and light. Delightfully balanced cereal and fruity notes. Volluto has an easy way about it.</t>
+  </si>
+  <si>
+    <t>VL1</t>
+  </si>
+  <si>
+    <t>Intenso</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446332870686/intenso-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/intenso_L.png</t>
+  </si>
+  <si>
+    <t>Vertuo</t>
+  </si>
+  <si>
+    <t>Long Coffee</t>
+  </si>
+  <si>
+    <t>230 ml (Coffee)</t>
+  </si>
+  <si>
+    <t>Smooth &amp; Strong</t>
+  </si>
+  <si>
+    <t>An intense long black coffee with a distinctly lingering aftertaste with roasted notes and a thick coffee crema. Pairs perfectly with milk that enriches the blend with brown caramel notes.</t>
+  </si>
+  <si>
+    <t>A blend of Nicaraguans washed Robusta coffee beans and Latin American Arabica. Thick with roasted notes and a lingering finish. The Arabicas get a darker roast to lower the acidity and bring out that brown sugar aroma. While the Nicaraguan coffee gets a longer roast to develop the Robusta coffee beans’ bold and bitter notes.</t>
+  </si>
+  <si>
+    <t>Intenso is created by combining Latin American Arabicas with Nicaraguan Robustas.</t>
+  </si>
+  <si>
+    <t>The Arabicas get a darker roast to lower the acidity and bring out that brown sugar aroma. The Robustas get a longer roast to develop bitter notes and a lingering aftertaste.</t>
+  </si>
+  <si>
+    <t>10 capsules of roast and ground coffee for the Nespresso system</t>
+  </si>
+  <si>
+    <t>125 g - 4.41 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL2</t>
+  </si>
+  <si>
+    <t>Stormio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446333558814/stormio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/stormio_L.png</t>
+  </si>
+  <si>
+    <t>Rich &amp; Strong</t>
+  </si>
+  <si>
+    <t>A long, slow roast intensifies the Nicaraguan and Guatemalan cereal aromatics to notes of spice and wood. They’re all high-grown Arabica coffees that we give that deep roast to build the rich intensity. But this Vertuo coffee pod remains smooth and full-bodied. Milk may mellow out Stormio - but you’ll still taste the powerful roasted notes that blow you away with a gathering storm.</t>
+  </si>
+  <si>
+    <t>Why we love it: Stormio’s a darkly roasted blend that rushes in with this myriad of aromas. But that all that strength could come from pure Arabica coffees?</t>
+  </si>
+  <si>
+    <t>125 g - 4.40 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL3</t>
+  </si>
+  <si>
+    <t>Odacio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446334378014/odacio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/odacio_XL.png</t>
+  </si>
+  <si>
+    <t>Bold &amp; Lively</t>
+  </si>
+  <si>
+    <t>The Nicaraguan Arabica gives Odacio its soft and solid cereal note. We daringly blended in a touch of Ethiopian Arabica - it adds a splash of acidity and delicate fruitiness. We split roast the coffees in this Vertuo coffee pod. A long and light roast for both coffees develops the body and structure and keeps the acidity and aromatics intact. Odacio brings a fullbodied cereal note and then dares to surprise you with its flourish of fruitiness and delicate acidity at the end. It’s bold and it’s lively and it hits your palate with great elegance.</t>
+  </si>
+  <si>
+    <t>Why we love it: Odacio’s a lively and intense Vertuo coffee.</t>
+  </si>
+  <si>
+    <t>VL4</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446443692062/mexico-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/mexico_L.png</t>
+  </si>
+  <si>
+    <t>Intense &amp; Spiced</t>
+  </si>
+  <si>
+    <t>Spicy &amp; Woody</t>
+  </si>
+  <si>
+    <t>An intense coffee with roasted woody and spicy notes, thick texture and low acidity. Pairs perfectly with milk.</t>
+  </si>
+  <si>
+    <t>You’ll do a double take with Master Origins Mexico with double washed Robusta -because selective hand-picking and thoroughly washing was once only for Arabica.</t>
+  </si>
+  <si>
+    <t>Both the Arabicas and Robustas from this coffee come from Mexico.</t>
+  </si>
+  <si>
+    <t>The Arabica coffee beans are given a medium roast and the uncommon Double Washed Robusta coffee beans get a long and deep roast.</t>
+  </si>
+  <si>
+    <t>VL5</t>
+  </si>
+  <si>
+    <t>Melozio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446335524894/melozio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/melozio_L.png</t>
+  </si>
+  <si>
+    <t>Smooth &amp; Balanced</t>
+  </si>
+  <si>
+    <t>A harmonious blend of Latin American Arabicas that sing with smooth cereal notes and a honeyed sweetness. Pairs perfectly with milk that enhances its softness and biscuity notes.</t>
+  </si>
+  <si>
+    <t>You can’t help but fall for Melozio, a Canadian best-seller. A harmonious blend of fine quality Brazilian and Central American Arabicas, roasted to create a rounded coffee that is smooth and perfectly balanced.</t>
+  </si>
+  <si>
+    <t>A harmonious blend of Latin American Arabicas, mostly from Brazil and Guatemala, rich in smooth cereal notes and honeyed sweetness.</t>
+  </si>
+  <si>
+    <t>The Brazilian Arabicas are roasted separately to develop sweet and cereal notes. The other Arabicas get are lightly roasted to round out Melozio.</t>
+  </si>
+  <si>
+    <t>VL6</t>
+  </si>
+  <si>
+    <t>Melozio Decaffeinato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446712553502/melozio-decaffeinato-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/melozio-decaffeinato_XL.png</t>
+  </si>
+  <si>
+    <t>Cereal</t>
+  </si>
+  <si>
+    <t>We split roast this Vertuo coffee capsule's Arabica coffees. It allows the Brazilian Bourbon to develop its cereal note to become a sweet and smooth coffee. Lightly roasting the other Arabicas rounds out Melozio. Melozio Decaffeinato delights twice. Its Latin American Arabicas still sing with smooth cereal and honeyed sweetness even after decaffeination.</t>
+  </si>
+  <si>
+    <t>Decaffeinated Roast and ground coffee.</t>
+  </si>
+  <si>
+    <t>VL7</t>
+  </si>
+  <si>
+    <t>Half Caffeinato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446338048030/half-caffeinato-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/half-caffeinato_L.png</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Velvety</t>
+  </si>
+  <si>
+    <t>This Vertuo coffee capsule blends decaffeinated and regular Arabica coffees from Brazil and Ethiopia. After decaffeination of half the coffee, a light and quick roast of a Brazilian Arabica coffee gives this Vertuo coffee pod a roundness and a sweetness. We chose to blend in an Ethiopian coffee so its delicate aromatics would add finesse. Half the coffee is Nespresso decaffeinated, but the taste is full.</t>
+  </si>
+  <si>
+    <t>Why we love it: You’ll love Half Caffeinato - its smooth, velvety texture and its sweet biscuit note.</t>
+  </si>
+  <si>
+    <t>VL8</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/26582353870878/el-salvador-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/el-salvador_2x.png?impolicy=medium&amp;imwidth=824&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Jam</t>
+  </si>
+  <si>
+    <t>Biscuity &amp; Winey</t>
+  </si>
+  <si>
+    <t>This coffee displays sweet, biscuity, fruity jam, and cereal notes, with a mild, low bitterness.</t>
+  </si>
+  <si>
+    <t>Grown under shade-trees, these treasured coffee varieties find their ideal terroir nestled beside active volcanoes, delivering a mild cup with sweet biscuit and fruity jam notes. The "red honey process" involves carefully adjusting the amount of sweet pulp left on the drying cherry which complements this Arabica blend’s washed processed beans with sweet aromatics.</t>
+  </si>
+  <si>
+    <t>This is an all-Arabica blend sourced from the Apaneca Ilamatepec Mountain Range in El Salvador. A selection of red honey processed beans complements the washed Arabica beans with distinctive sweetness.</t>
+  </si>
+  <si>
+    <t>Overall light roast - The red honey is roasted separately from the rest to make the most of the unique processing method. The other portion washed is slightly longer and darker.</t>
+  </si>
+  <si>
+    <t>VL9</t>
+  </si>
+  <si>
+    <t>Colombia - Fairtrade</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446444412958/colombia-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/13252876304414/C-0369-Main-PDP-MasterOrigin-Colombia-VL.jpg?impolicy=productPdpSafeZone&amp;imwidth=1238</t>
+  </si>
+  <si>
+    <t>Red fruit notes</t>
+  </si>
+  <si>
+    <t>The longer fermentation of high-grown Colombian Arabica delivers a particularly juicy and fruity, sweet cup. Pairs perfectly with milk.</t>
+  </si>
+  <si>
+    <t>The cooler climate of the high-altitude Colombia Aguadas mountains means the coffee takes longer to ferment. The classic washed coffee processing method is complex and time-consuming, but up here it calls for even more skill.</t>
+  </si>
+  <si>
+    <t>This fully-washed coffee is sourced in the high-altitude region of Aguadas, in Colombia.</t>
+  </si>
+  <si>
+    <t>We separate this coffee in 2 batches for roasting. Most of it is given a fast and light roast, and a smaller portion is roasted a little longer and deeper to add complexity to the cup.</t>
+  </si>
+  <si>
+    <t>VL10</t>
+  </si>
+  <si>
+    <t>Solelio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446443167774/solelio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/solelio_L.png</t>
+  </si>
+  <si>
+    <t>Fruity &amp; Lightly-bodied</t>
+  </si>
+  <si>
+    <t>Cereal &amp; Fruity</t>
+  </si>
+  <si>
+    <t>This Vertuo coffee capsule is an Arabica blend of two renowned washed coffees - both loved for their lively acidity and their distinct fruity notes. We split roast and blended high-grown Colombian coffee and Kenyan coffee to create a light roast coffee with a light body and a lovable character. A juicy acidity shines through Solelio’s toasted cereal note. It’s hard to miss the classic fruitiness of the Colombian and Kenyan coffees. You can really ease into morning with this Vertuo coffee.</t>
+  </si>
+  <si>
+    <t>Why we love it: Solelio is our gentlest start to the day.</t>
+  </si>
+  <si>
+    <t>VL11</t>
+  </si>
+  <si>
+    <t>Alto Onice</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/28487841939486/Alto-Onice-PLP.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/alto-onice_2x.png</t>
+  </si>
+  <si>
+    <t>Long Coffee — Exclusively for use with Vertuo Next, Vertuo Pop+, Vertuo Lattissima and Vertuo Creatista machines</t>
+  </si>
+  <si>
+    <t>355 ml (Alto)</t>
+  </si>
+  <si>
+    <t>Roasted, Woody &amp; Spicy</t>
+  </si>
+  <si>
+    <t>An intense coffee with roasted, woody and spicy notes.</t>
+  </si>
+  <si>
+    <t>Alto Onice delivers a full palate of strong cereal and deep woody notes for a longer cup to savour at home or on-the-go. Through the bold aromatics of beautiful bitter cocoa, spice and roasted notes comes a golden caramel note and a faint shimmer of acidity to balance this deep-roasted blend of coffees from Colombia, India, and beyond.</t>
+  </si>
+  <si>
+    <t>A complex blend of several origins: through its Indian beans’ cocoa and spice notes comes the Colombian arabica’s shimmer of acidity in our longest cup size.</t>
+  </si>
+  <si>
+    <t>Arabicas and robustas are roasted together in the first split. The second split is composed exclusively from decaffeinated arabica, and is roasted for a slightly shorter time.</t>
+  </si>
+  <si>
+    <t>7 capsules of roast and ground coffee for the Nespresso system.</t>
+  </si>
+  <si>
+    <t>Roast and ground coffee, decaffeinated roast and ground coffee.</t>
+  </si>
+  <si>
+    <t>120 g - 4.23 oz for 7 capsules</t>
+  </si>
+  <si>
+    <t>VL12</t>
+  </si>
+  <si>
+    <t>Alto Ambrato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/28487841415198/Alto-Ambrato-PLP.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/alto-ambrato_2x.png</t>
+  </si>
+  <si>
+    <t>Honeyed &amp; Delicate</t>
+  </si>
+  <si>
+    <t>Cereal &amp; Honey</t>
+  </si>
+  <si>
+    <t>Ambrato is a delicate blend with light toasted bread and honey notes and a light body.</t>
+  </si>
+  <si>
+    <t>Taste Alto Ambrato's honeyed cereal, toasted notes and caramel sweetness. A fruity touch sparkles through this lightly roasted blend of fine Latin American Arabicas and Robusta. At home or on the go, it’s your longer cup warm in rich, golden aromatics.</t>
+  </si>
+  <si>
+    <t>Arabica and robusta coffees from Latin America give rich warmth to this light-roast long cup. Taste toasted cereal and sweet caramel notes balanced by a fruity touch.</t>
+  </si>
+  <si>
+    <t>VL13</t>
+  </si>
+  <si>
+    <t>Cold Brew Style Intense</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/26731415470110/cold-brew-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/cold-brew-intense.png</t>
+  </si>
+  <si>
+    <t>355 ml (Cold Brew)</t>
+  </si>
+  <si>
+    <t>Sweet Caramel &amp; Roasted Cereal</t>
+  </si>
+  <si>
+    <t>Caramel &amp; Roasted Cereal</t>
+  </si>
+  <si>
+    <t>A smooth and silky-textured coffee, with roasted caramel notes, low bitterness and a pleasant acidity that is typical of cold brew extractions.</t>
+  </si>
+  <si>
+    <t>Inspired by the “hot bloom” method, Cold Brew Style Intense, reimagined by Nespresso, begins brewing hot to draw the best of the beans &amp; continues with cool water to leave the bitterness behind and brewed in minutes. Taste the roasted Arabicas’ &amp; caramel notes in a smooth, silky-textured coffee. For the best experience, use cool water (below 10°C / 50F) in your Vertuo water tank &amp; add 3-4 ice cubes to your coffee. 12 fl oz (355 ml) = 2 servings of 6 fl oz (172.5 ml).</t>
+  </si>
+  <si>
+    <t>This 100% Arabica blend mostly uses Brazilian Bourbons and other Guatemalan Arabicas.</t>
+  </si>
+  <si>
+    <t>This Vertuo coffee gets a split roast. It allows the Brazilian Bourbon to develop its cereal note to become a sweet and smooth coffee. Lightly roasting the other Arabicas rounds out the blend.</t>
+  </si>
+  <si>
+    <t>7 Cold Brew Style Intense capsules of roast and ground coffee for the Nespresso system.</t>
+  </si>
+  <si>
+    <t>VL14</t>
+  </si>
+  <si>
+    <t>Carafe Pour-Over Style</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17299762282526/carafe-pour-over-style-intense-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/carafe-pour-over-style_L.png</t>
+  </si>
+  <si>
+    <t>Long Coffee — Exclusively for use with Vertuo Next, Vertuo Lattissima and Vertuo Creatista machines</t>
+  </si>
+  <si>
+    <t>535 ml (Carafe)</t>
+  </si>
+  <si>
+    <t>Roasted &amp; Smokey</t>
+  </si>
+  <si>
+    <t>CARAFE POUR-OVER STYLE is the coffee that opens up possibilities for sharing with others or simply extending the pleasure of your Nespresso moment. But creating our longest cup was by no means our shortest journey. Delivering not just the right intensity in the 535 ml, but also optimum crema and a distinct flavour profile, is something that didn’t happen overnight. After years of development, we were able to refine &amp; perfect the product to our desire, welcoming our largest ever coffee into the family. Elevate your drinking experience with the CARAFE accessory set, specifically designed to reveal the coffee's unique aromatics and inspire a new Nespresso coffee ritual.</t>
+  </si>
+  <si>
+    <t>CARAFE POUR-OVER SYLE is a coffee like none other in the range. It’s an easy-to-drink blend of Peruvian and Colombian washed Arabicas, which complement each other with their contrasting qualities to create a unique aromatic profile.</t>
+  </si>
+  <si>
+    <t>7 capsules of roast and ground coffee for the Vertuo Next Machine.</t>
+  </si>
+  <si>
+    <t>Roast and ground coffee.</t>
+  </si>
+  <si>
+    <t>VL15</t>
+  </si>
+  <si>
+    <t>Carafe Pour-Over Style Mild</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17299762511902/carafe-pour-over-style-mild-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15890435342366/Untitled-11.png</t>
+  </si>
+  <si>
+    <t>Toasted Cereal &amp; Malted</t>
+  </si>
+  <si>
+    <t>Round and easy to drink, Carafe Pour-Over Style Mild has a balanced sensorial profile with toasted cereal notes and pleasant sweetness. This blend was roasted using the split roast technique (60/40). The first split includes all origins and is roasted to a light degree and average roasting time, while their second split includes only Colombian coffees and is roasted to a slightly darker degree, creating a mild roast overall. A classic Vertuo roast.</t>
+  </si>
+  <si>
+    <t>Smooth, toasted cereal and malted notes grace every last drop of this subtly sweet Latin American Arabica blend coffee inspired by the pour-over method.</t>
+  </si>
+  <si>
+    <t>VL16</t>
+  </si>
+  <si>
+    <t>Fortado</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14463427837982/fortado-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/fortado_L.png</t>
+  </si>
+  <si>
+    <t>Gran Lungo</t>
+  </si>
+  <si>
+    <t>150 ml (Gran Lungo)</t>
+  </si>
+  <si>
+    <t>Intense &amp; Full-bodied</t>
+  </si>
+  <si>
+    <t>Cocoa</t>
+  </si>
+  <si>
+    <t>The most intense coffee in its Gran Lungo size comes thick-bodied and full of cocoa and oak notes. Pairs perfectly with milk.</t>
+  </si>
+  <si>
+    <t>Here’s the most intense Vertuo coffee in its Gran Lungo size - Fortado. Its Indian Robusta comes at you in full force, and cocoa and oak wood notes emerge from the Latin American Arabicas.</t>
+  </si>
+  <si>
+    <t>We chose high quality washed Latin American Arabicas and blended it with a naturally processed Indian Robusta for its high-end quality, intensity and full body.</t>
+  </si>
+  <si>
+    <t>First, a long roast at medium temperatures brings out the intensity in the Indian Robusta, without any harshness. The Arabicas then get dark developing rich cocoa and wood notes.</t>
+  </si>
+  <si>
+    <t>100 g - 3.53 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL17</t>
+  </si>
+  <si>
+    <t>Fortado Decaffeinato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446710554654/fortado-decaffeinato-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/fortado-decaffeinato_L.png</t>
+  </si>
+  <si>
+    <t>Woody</t>
+  </si>
+  <si>
+    <t>The thick-bodied character with cocoa and oak notes of Fortado, in a decaffeinated recipe. Pairs perfectly with milk.</t>
+  </si>
+  <si>
+    <t>The most intense Gran Lungo VERTUO coffee, decaffeinated. FORTADO DECAFFEINATO’s Indian Robusta comes at you in full force, with cocoa and oak wood notes still strong in the decaffeinated Latin American Arabicas.</t>
+  </si>
+  <si>
+    <t>VL18</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446316486686/costa-rica-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/costa-rica_L.png</t>
+  </si>
+  <si>
+    <t>Malty &amp; Cereal Notes</t>
+  </si>
+  <si>
+    <t>The one-of-a-kind process of fermentation in hot-spring waters brings about a remarkably balanced and clean taste in the cup. Master Origins Costa Rica is full-bodied but mellow. A malty sweet cereal note runs through it with crystal clarity.</t>
+  </si>
+  <si>
+    <t>High in Costa Rica’s mountains, only a small selection of Arabica coffee beans is soaked in rainforest hot spring waters. Costa Rica contains this scarce coffee whose rare process highlights the malty sweet cereal character of this craftsman’s coffee.</t>
+  </si>
+  <si>
+    <t>This 100% Arabica, fully washed coffee is sourced high up in the Costa Rican mountains.</t>
+  </si>
+  <si>
+    <t>First batch is roasted in medium temperatures to reach a medium-dark colour and develop sweet malty notes. Second batch is roasted more intensively to reach a darker color and the desired intensity.</t>
+  </si>
+  <si>
+    <t>105 g - 3.70 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL19</t>
+  </si>
+  <si>
+    <t>Arondio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446108835870/arondio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/arondio_L.png</t>
+  </si>
+  <si>
+    <t>Cereal &amp; Mild</t>
+  </si>
+  <si>
+    <t>A mild Gran Lungo - but don’t be fooled - there’s an inner strength behind the cereal note - a subtle acidity and a hint of Robusta oomph. The addition of milk softens the cereal notes while keeping an enchanting character.</t>
+  </si>
+  <si>
+    <t>VL20</t>
+  </si>
+  <si>
+    <t>Inizio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446709669918/inizio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/inizio_L.png</t>
+  </si>
+  <si>
+    <t>Floral &amp; Cereal</t>
+  </si>
+  <si>
+    <t>Floral</t>
+  </si>
+  <si>
+    <t>We split roast this medium roast coffee. The Ethiopian Arabicas get a lighter, shorter roast to keep those floral notes alive. A longer, darker roast of the Kenyan coffee adds body to this Vertuo coffee capsule. The brewing is also designed to bring out great crema while keeping the floral aromatics intact. A juicy coffee with that combines subtle floral and cereal notes.</t>
+  </si>
+  <si>
+    <t>Inizio is the helping hand easing you into your every day. The velvety, smooth body of this Kenyan and Ethiopian Arabica blend comes with a warmth and strength from its rich toasted cereal note. Its wild florals give you that laid-back Sunday feeling.</t>
+  </si>
+  <si>
+    <t>VL21</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446318485534/ethiopia-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/ethiopia_XL.png</t>
+  </si>
+  <si>
+    <t>Floral &amp; Delicate</t>
+  </si>
+  <si>
+    <t>Ethiopia is a naturally flowery coffee that gains fruitiness and complexity from its signature drying method, revealing ripe blueberry notes and a hint of musk.</t>
+  </si>
+  <si>
+    <t>Ethiopia with dry processed Arabica involves sun-drying some of the coffee cherry. This continual hand-turning to ensure even drying calls for great care. And Ethiopian farmers have used this method for longer than anyone else.</t>
+  </si>
+  <si>
+    <t>95 g - 3.35 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL22</t>
+  </si>
+  <si>
+    <t>Il Caffe</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446323925022/il-caffe-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15537109106718/il-caffe-XL.png</t>
+  </si>
+  <si>
+    <t>Espresso</t>
+  </si>
+  <si>
+    <t>Exceptionally Intense &amp; Velvety</t>
+  </si>
+  <si>
+    <t>Cereal, Woody &amp; Cocoa</t>
+  </si>
+  <si>
+    <t>We split roast the coffees to give the Robustas a darker roast. A lighter but slightly longer roast of the Colombian Arabica beans keeps the acidity intact and develops a hint of a nutty note. Il Caffè goes down like a dream, its classic aroma promises to delight, and its familiar flavour is one to remember. We crafted Il Caffè to be your traditional black coffee experience, but if you want to soften this one’s intensity, why not add milk to make a Cappuccino?</t>
+  </si>
+  <si>
+    <t>70 g - 2.47 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL23</t>
+  </si>
+  <si>
+    <t>Diavolitto</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446103330846/diavolitto-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/diavolitto_L.png</t>
+  </si>
+  <si>
+    <t>Highly Intense &amp; Powerful</t>
+  </si>
+  <si>
+    <t>Intense &amp; Woody</t>
+  </si>
+  <si>
+    <t>No harshness in Diavolitto - just fine oak wood and leather notes and a smooth, creamy texture. The addition of milk complements its natural full body.</t>
+  </si>
+  <si>
+    <t>This short devil of a coffee capsule is an intense, powerful espresso, definitely packed with character. Oak and leather aromas punch through the creamy texture of Diavolitto's blend of Robustas, including washed Guatemalan Robusta, and Latin American Arabicas.</t>
+  </si>
+  <si>
+    <t>A blend of Robustas and Arabicas from Latin America and a rare Robusta from Guatemala which gives to this coffee its soft and creamy texture.</t>
+  </si>
+  <si>
+    <t>A highly roasted Robusta and Arabica coffee blend. We split roast so that each coffee’s origin characteristics stay at play.</t>
+  </si>
+  <si>
+    <t>VL24</t>
+  </si>
+  <si>
+    <t>Altissio Decaffeinato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446707310622/altissio-decaffeinato-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/altissio-decaffeinato_XL.png</t>
+  </si>
+  <si>
+    <t>Full-bodied &amp; Creamy</t>
+  </si>
+  <si>
+    <t>The full-bodied, bold espresso taste comes from blending South American Arabicas with Robusta. A Costa Rican Arabica adds its soft cereal note. All decaffeinated, the taste of the highly roasted Altissio Decaffeinato is true to the original – still cloaked in creamy royal robes.</t>
+  </si>
+  <si>
+    <t>When Altissio Decaffeinato walks in, you'll notice.</t>
+  </si>
+  <si>
+    <t>70 g - 2.46 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL25</t>
+  </si>
+  <si>
+    <t>Altissio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446104018974/altissio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/altissio_XL.png?impolicy=medium&amp;imwidth=824&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>Full-Bodied &amp; Creamy</t>
+  </si>
+  <si>
+    <t>A bold espresso cloaked in a creamy and roasty cereal note. Pairs perfectly with milk that complements its natural full body.</t>
+  </si>
+  <si>
+    <t>The South American Arabicas and a touch of Brazilian Robusta give it that full-bodied, bold espresso taste. We balanced these coffees out with a Costa Rican Arabica that adds its soft cereal note. In royal robes, Altissio is a Vertuo espresso coffee cloaked in a thick, velvety crema - full of roasty notes and a soft and creamy cereal note.</t>
+  </si>
+  <si>
+    <t>A combination of Arabicas from Latin America and Costa Rica, with a little touch of Brazilian Robusta for a full-bodied cup.</t>
+  </si>
+  <si>
+    <t>Altissio gets an intense and short roast to bring out the full-bodied character of this bold Vertuo espresso coffee.</t>
+  </si>
+  <si>
+    <t>VL26</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446106738718/peru-organic-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15536827269150/peru-oranic-vl-L.png</t>
+  </si>
+  <si>
+    <t>High up above 1000 meters – even up to 2100 meters – and, tucked into the slopes of the Andes, we found them. The organic processes passed down from generation to generation, this coffee is blessed with the meticulous care of smallholder farmers. Peru Organic is split roast to reveal both the bright, juicy acidity and the elegant fruity notes accented by a smooth toasted cereal note.</t>
+  </si>
+  <si>
+    <t>Why we love it: We traveled across remote Peruvian regions in search of the finest organic certified Arabica coffee beans.</t>
+  </si>
+  <si>
+    <t>VL27</t>
+  </si>
+  <si>
+    <t>Orafio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446706262046/orafio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/orafio_L.png</t>
+  </si>
+  <si>
+    <t>Caramel &amp; Roasted</t>
+  </si>
+  <si>
+    <t>Caramel</t>
+  </si>
+  <si>
+    <t>We crafted Orafio with a light and long roasted Ugandan Robusta. That roast keeps this coffee’s typical body and bitterness in check while still delivering the liquorice and spice notes that are hallmarks of this origin’s naturally processed Robusta. A short dark roast of the Brazilian and Costa Rican Arabicas balances the blend. Orafio is a complex coffee carrying a delicious caramel note and lingering with a long finish. Its beautiful roasted notes graced by a hint of acidity make this a luxurious coffee worth its weight in gold.</t>
+  </si>
+  <si>
+    <t>What makes Orafio glow in your cup is a combination of masterful blending, bringing together both high quality Arabica and Robusta coffees from a diversity of origins, and skilful split roasting. Sounds a bit like the level of craftmanship that goes into this coffee’s namesake, doesn’t it? The Italians among us will recognize the link to their word for goldsmith.</t>
+  </si>
+  <si>
+    <t>62 g - 2.18 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL28</t>
+  </si>
+  <si>
+    <t>Toccanto</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17299757563934/toccanto-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/toccanto_XL.png?impolicy=medium&amp;imwidth=824&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>Berry &amp; Winey</t>
+  </si>
+  <si>
+    <t>Fill your cup with the wildly aromatic Toccanto - a juicy coffee whose Latin American Arabicas bring candied and winey fruit notes to your palate.</t>
+  </si>
+  <si>
+    <t>A barrel of fine South and Central American coffee origins gather together in Toccanto to bring you a wild, juicy coffee with candied and ripe fruity notes. This all Arabica blend beautifully balances acidity and body in an aromatic cup.</t>
+  </si>
+  <si>
+    <t>VL29</t>
+  </si>
+  <si>
+    <t>Voltesso</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446104870942/voltessio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>Light &amp; Sweet</t>
+  </si>
+  <si>
+    <t>A sweet, mild and harmonious blend with delicate biscuity aromas. Perfectly pairs with a dash of milk if you are looking for an even smoother taste.</t>
+  </si>
+  <si>
+    <t>Our light and sweet espresso that comes with a biscuity aroma from its fine South American Arabicas and that you might just make your golden standard.</t>
+  </si>
+  <si>
+    <t>Voltesso gets its light, biscuity note from Brazilian Bourbon coffee, while Colombian Arabicas add a hint of acidity.</t>
+  </si>
+  <si>
+    <t>The Colombian coffee is roasted light and short to preserve its acidity, while the Brazilian Bourbon is roasted for a longer time to reveal its biscuity notes.</t>
+  </si>
+  <si>
+    <t>52 g - 1.83 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL30</t>
+  </si>
+  <si>
+    <t>Double Espresso Scuro</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446108147742/double-espresso-scuro-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/double-espresso-scuro_XL.png</t>
+  </si>
+  <si>
+    <t>80 ml (Double Espresso)</t>
+  </si>
+  <si>
+    <t>Dark &amp; Bold</t>
+  </si>
+  <si>
+    <t>A highly roasted blend of both Arabica and Robusta, that gives to Double Espresso Scuro a smoky character with dark cocoa and subtle vanilla notes. Pairs perfectly with milk.</t>
+  </si>
+  <si>
+    <t>Double Espresso Scuro is a highly roasted blend of Robusta and Arabica - all Central American coffees. The Robusta is from Guatemala and the Arabica is Costa Rican. And it’s the Robusta in this Nespresso Vertuoline double shot that helps it pack a double enjoyment.</t>
+  </si>
+  <si>
+    <t>This intense blend is created using Robustas from Guatemala and other origins, in combination with Arabicas from Costa Rica.</t>
+  </si>
+  <si>
+    <t>We separate Robustas and Arabicas but give them both a full roast to develop the intense cocoa notes and the smoky character of this coffee.</t>
+  </si>
+  <si>
+    <t>100 g - 3.52 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL31</t>
+  </si>
+  <si>
+    <t>Double Espresso Chiaro</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446107885598/double-espresso-chiaro-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/double-espresso-chiaro_XL.png?impolicy=medium&amp;imwidth=824&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>Dense &amp; Wild</t>
+  </si>
+  <si>
+    <t>An intense yet balanced Double Espresso, with woody, earthy and roasted cereal notes. Pairs perfectly with milk that enriches the blend with surprisingly prominent notes of caramel.</t>
+  </si>
+  <si>
+    <t>This Nespresso Vertuoline double shot’s the last course - go ahead and finish off your meal with a bang.</t>
+  </si>
+  <si>
+    <t>A blend of Latin American Arabica coffees, mainly coming from Brazil and Colombia.</t>
+  </si>
+  <si>
+    <t>Washed and Natural Arabicas are roasted separately, although both get an intense and short roast. This is done to bring the best out of each part of the blend.</t>
+  </si>
+  <si>
+    <t>VL32</t>
+  </si>
+  <si>
+    <t>Double Espresso Dolce</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446713602078/double-espresso-dolce-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/double-espresso-dolce_L.png</t>
+  </si>
+  <si>
+    <t>Cereal &amp; Malted</t>
+  </si>
+  <si>
+    <t>An exceptionally smooth double espresso that gets its sweetness and malty toasted cereal notes from a fine blend of Arabica and Robusta. Pairs perfectly with milk.</t>
+  </si>
+  <si>
+    <t>The masterful blending and split roasting of different Arabica and Robusta beans is the secret behind this mild and smooth double espresso. Latin American Arabicas deliver that delicious malty toasted cereal note that sings above this beautifully balanced cup.</t>
+  </si>
+  <si>
+    <t>Double Espresso Dolce is created by combining Latin American Arabicas and Ugandan Robustas.</t>
+  </si>
+  <si>
+    <t>A batch of Arabicas are roasted light and short, while another combination of Arabica and Robusta get a slightly longer and darker roast.</t>
+  </si>
+  <si>
+    <t>VL33</t>
+  </si>
+  <si>
+    <t>Roasted Hazelnut</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17452241649694/roasted-hazelnut-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/roasted-hazelnut_2x.png</t>
+  </si>
+  <si>
+    <t>230 ml (Coffee), Cappucino and Latte Macchiato</t>
+  </si>
+  <si>
+    <t>Hazelnut &amp; Flavoured</t>
+  </si>
+  <si>
+    <t>This flavoured blend delights with its classic grilled hazelnut flavour, complemented by notes of biscuits and caramel.</t>
+  </si>
+  <si>
+    <t>We have made name changes to our Barista Creations flavoured range for Vertuo to better reflect the various changes made, from the recipe to the flavouring extracts and recommended cup size. Bringing you the rich caramelized flavour of roasted hazelnuts in a coffee called for perfectly roasting some of our smoothest Arabica beans from Latin America and Africa. When this sweet, velvety blend with its delicate biscuit note meets the bittersweet complexity of the hazelnut flavour in Barista Creations Flavoured Roasted Hazelnut it’s all smiles. It makes a milky treat with a rush of grilled hazelnut, praline, and caramel biscuit notes.</t>
+  </si>
+  <si>
+    <t>This 100% Arabica blend is sourced from Brazil and Ethiopia and another Latin American Country.</t>
+  </si>
+  <si>
+    <t>Latin American beans are roasted medium dark and quickly to develop sweetness. The other coffees are roasted a bit longer to develop a velvety texture.</t>
+  </si>
+  <si>
+    <t>10 capsules of artificially flavoured hazelnut roast and ground coffee for the Nespresso system.</t>
+  </si>
+  <si>
+    <t>VL34</t>
+  </si>
+  <si>
+    <t>Golden Caramel</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17452249612318/golden-caramel-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/golden-caramel.png</t>
+  </si>
+  <si>
+    <t>Caramel &amp; Flavoured</t>
+  </si>
+  <si>
+    <t>This flavoured blend delights with the classic caramel flavour combined with sweet biscuit notes.</t>
+  </si>
+  <si>
+    <t>We have made name changes to our Barista Creations flavoured range for Vertuo to better reflect the various changes made, from the recipe to the flavouring extracts and recommended cup size. Barista Creations Flavoured Golden Caramel brings the weekend mood any day. Into our sweet and velvety base blend of Latin American and African Arabicas comes the comforting caramel flavour. Its biscuity sweetness is an echo of the coffee blend itself, this one’s got layers of indulgence irresistibly inviting you to cozy up any time the moment calls for it. Insider Tip: With a dash of milk, the caramel and biscuit notes can’t be missed.</t>
+  </si>
+  <si>
+    <t>VL35</t>
+  </si>
+  <si>
+    <t>Sweet Vanilla</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17452245155870/sweet-vanilla-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/sweet-vanilla_2x.png</t>
+  </si>
+  <si>
+    <t>Vanilla &amp; Flavoured</t>
+  </si>
+  <si>
+    <t>This flavoured blend delights with the classic vanilla flavour combined with sweet biscuit, candied and cereal notes coming from its delicate arabica base.</t>
+  </si>
+  <si>
+    <t>We have made name changes to our Barista Creations flavoured range for Vertuo to better reflect the various changes made, from the recipe to the flavouring extracts and recommended cup size.Tuck into Barista Creations Flavoured Sweet Vanilla - the dreamy taste of vanilla dances through delicious coffee. When we add vanilla flavour to our light-roasted Arabicas from Latin America and Africa, you’ll discover much more in the cup. It takes on a swirl of flavours. Notes of caramel and vanilla cake are all the excuse you need to pause and enjoy a little me-time. Just for you or to share with loved ones. Insider tip: A dash of milk highlights the vanilla flavour all the more.</t>
+  </si>
+  <si>
+    <t>10 capsules of roast and ground coffee for the Nespresso system. Vanilla flavour with other natural flavours.</t>
+  </si>
+  <si>
+    <t>Roast and ground coffee, natural flavour.</t>
+  </si>
+  <si>
+    <t>VL36</t>
+  </si>
+  <si>
+    <t>Rich Chocolate</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/17452242108446/rich-chocolate-2x.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/global/coffees/vl/sku-main-info-product/rich-chocolate_2x.png?impolicy=medium&amp;imwidth=824&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>Dark Chocolate Flavoured</t>
+  </si>
+  <si>
+    <t>Chocolate &amp; Flavoured</t>
+  </si>
+  <si>
+    <t>This flavoured blend delights with its elegant dark chocolate flavour, complemented by notes of caramel, almond and cereal.</t>
+  </si>
+  <si>
+    <t>Satisfy your chocolate craving with BARISTA CREATIONS FLAVOURED RICH CHOCOLATE. Our velvety-smooth blend of Latin American and African Arabicas meets an authentic chocolate flavour, inviting you to make an occasion of your coffee moment. Like all good dark chocolate—rich and complex—this coffee unfolds layers of flavour. The sweetness elevates it to dessert status. Insider tip: With a dash of milk, a rush of nuts and biscuit notes emerges to accompany the chocolate flavour.</t>
+  </si>
+  <si>
+    <t>10 capsules of flavoured roast and ground coffee for the Nespresso system.</t>
+  </si>
+  <si>
+    <t>Roast and ground coffee. Cocoa flavour with other natural flavours.</t>
+  </si>
+  <si>
+    <t>VL37</t>
+  </si>
+  <si>
+    <t>Bianco Piccolo</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15916187648030/C-1035-ResponsivePLPImage.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/bianco-piccolo/bianco-piccolo.png</t>
+  </si>
+  <si>
+    <t>40 ml (Espresso) &amp; Milk Recipes</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Smooth</t>
+  </si>
+  <si>
+    <t>Smooth &amp; Sweet</t>
+  </si>
+  <si>
+    <t>Soft and smooth, creamy texture, sweet, notes of caramel, nuts and biscuit. Especially crafted for your recipes with milk.</t>
+  </si>
+  <si>
+    <t>Intense yet smooth in taste, this espresso is specially designed for making cappuccinos, latte macchiatos or flat whites. An expertly crafted blend of Arabicas from China, Colombia, Brazil &amp; Ethiopia creates this world of rich roasted notes to land in harmony with the creamy sweetness of milk.</t>
+  </si>
+  <si>
+    <t>For this 100% Arabica blend, we sourced beans from a diversity of origins stretching from China to Colombia, and Brazil to Ethiopia.</t>
+  </si>
+  <si>
+    <t>Roasted in two splits : 1. Medium-dark for the majority of the coffee. 2. Light to very light to balance out the overall roast, aiming for the best combination to work well with milk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roast and ground coffee </t>
+  </si>
+  <si>
+    <t>62 g - 2.19 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL38</t>
+  </si>
+  <si>
+    <t>Bianco Doppio</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15922851577886/C-1034-ResponsivePLPImage.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/bianco-doppio/bianco-doppio.png</t>
+  </si>
+  <si>
+    <t>80 ml (Double Espresso) &amp; Milk Recipes</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Milky</t>
+  </si>
+  <si>
+    <t>A smooth and caramelly light-roast Arabica blend crafted specifically for your larger milky coffees.</t>
+  </si>
+  <si>
+    <t>We crafted this coffee as the match for your longer milky treats. An aromatic blend of light roasted Arabicas from Kenya, Colombia and Nicaragua, our signature split roast develops delicious caramelly notes and a smooth texture in BIANCO DOPPIO for milk. It’s the coffee that pairs beautifully with milk in your larger cappuccinos and flat whites.</t>
+  </si>
+  <si>
+    <t>The majority of the coffee goes on a very light first split, while the second split is pushed a bit further. A very clear and light roast overall.</t>
+  </si>
+  <si>
+    <t>102 g - 3.59 oz for 10 capsules</t>
+  </si>
+  <si>
+    <t>VL39</t>
+  </si>
+  <si>
+    <t>Bianco Forte</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16058298040350/C-0290-ResponsivePLPImage.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/bianco-forte/bianco-forte.png</t>
+  </si>
+  <si>
+    <t>Balanced &amp; Intense</t>
+  </si>
+  <si>
+    <t>A full-bodied, intense and dark-roasted coffee, rich in cereal notes. Especially crafted for your recipes, it remains powerful in combination with milk.</t>
+  </si>
+  <si>
+    <t>A long cup coffee, big in powerful roasted notes. Add a generous dash of milk and you’ll find its sweetness sits in a dynamic balance with this carefully crafted blend of fine Colombian and Kenyan Arabicas. We give the beans a dark split roast to highlight the coffees' rich roasted and cereal notes.</t>
+  </si>
+  <si>
+    <t>This 100% Arabica blend combines coffees from Kenya, Colombia and Costa Rica.</t>
+  </si>
+  <si>
+    <t>One part of the blend gets a long and dark roast, while the second part is roasted a little faster and to a slightly lighter degree.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1163,8 +2234,13 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1189,6 +2265,12 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -1196,7 +2278,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1229,6 +2311,12 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1449,9 +2537,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.13"/>
-    <col customWidth="1" min="2" max="2" width="19.38"/>
+    <col customWidth="1" min="2" max="2" width="21.88"/>
     <col customWidth="1" min="5" max="5" width="6.75"/>
-    <col customWidth="1" min="6" max="6" width="6.5"/>
+    <col customWidth="1" min="6" max="6" width="8.0"/>
     <col customWidth="1" min="7" max="7" width="15.0"/>
     <col customWidth="1" min="8" max="8" width="13.63"/>
     <col customWidth="1" min="10" max="10" width="7.25"/>
@@ -4156,6 +5244,2814 @@
       <c r="AA37" s="4" t="s">
         <v>110</v>
       </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="J38" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="N38" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O38" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P38" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="W38" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="X38" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="Y38" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="Z38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA38" s="4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J39" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="N39" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O39" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P39" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y39" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA39" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J40" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="N40" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="O40" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P40" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y40" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA40" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="J41" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="N41" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O41" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P41" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="W41" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="Y41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="J42" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="K42" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="N42" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O42" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P42" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="W42" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="X42" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y42" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA42" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="J43" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="K43" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="N43" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O43" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P43" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="Y43" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z43" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA43" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="J44" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="N44" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O44" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P44" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="Y44" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J45" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="N45" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="O45" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P45" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="X45" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="Y45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA45" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="J46" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="N46" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="O46" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P46" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="Y46" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="J47" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="N47" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O47" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P47" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="Y47" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J48" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="K48" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="N48" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O48" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P48" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="X48" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="Y48" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="Z48" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="AA48" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="J49" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="K49" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O49" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P49" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="10"/>
+      <c r="V49" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="W49" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="X49" s="7"/>
+      <c r="Y49" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="Z49" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="AA49" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K50" s="2">
+        <v>10.85</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="10"/>
+      <c r="V50" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="W50" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="X50" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="Y50" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="Z50" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="AA50" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K51" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="L51" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="N51" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O51" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P51" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y51" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="Z51" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA51" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K52" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="L52" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="N52" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O52" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P52" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="10"/>
+      <c r="U52" s="10"/>
+      <c r="V52" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="Y52" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="Z52" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA52" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="J53" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="K53" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="N53" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O53" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P53" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10"/>
+      <c r="U53" s="10"/>
+      <c r="V53" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="W53" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="X53" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="Y53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z53" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA53" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="J54" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="K54" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="N54" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O54" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P54" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10"/>
+      <c r="U54" s="10"/>
+      <c r="V54" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="W54" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="X54" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="Y54" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z54" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA54" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="J55" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="K55" s="2">
+        <v>12.1</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="N55" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O55" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P55" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R55" s="10"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10"/>
+      <c r="U55" s="10"/>
+      <c r="V55" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="W55" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="X55" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="Y55" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z55" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA55" s="4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="J56" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="K56" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L56" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="N56" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O56" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P56" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
+      <c r="U56" s="10"/>
+      <c r="Y56" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z56" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA56" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="J57" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="K57" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="N57" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O57" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P57" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q57" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="R57" s="10"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="10"/>
+      <c r="U57" s="10"/>
+      <c r="V57" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y57" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z57" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA57" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="J58" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="K58" s="2">
+        <v>12.1</v>
+      </c>
+      <c r="L58" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="N58" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O58" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P58" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="10"/>
+      <c r="U58" s="10"/>
+      <c r="V58" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="Y58" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z58" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA58" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="J59" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="K59" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="N59" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O59" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P59" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R59" s="10"/>
+      <c r="S59" s="10"/>
+      <c r="T59" s="10"/>
+      <c r="U59" s="10"/>
+      <c r="V59" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="Y59" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z59" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA59" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="J60" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="K60" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="N60" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O60" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="P60" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="R60" s="10"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="10"/>
+      <c r="U60" s="10"/>
+      <c r="V60" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="W60" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="X60" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="Y60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z60" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA60" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="J61" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="K61" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="N61" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O61" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P61" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R61" s="10"/>
+      <c r="S61" s="10"/>
+      <c r="T61" s="10"/>
+      <c r="U61" s="10"/>
+      <c r="V61" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="Y61" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z61" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA61" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="J62" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="K62" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="N62" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O62" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P62" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R62" s="10"/>
+      <c r="S62" s="10"/>
+      <c r="T62" s="10"/>
+      <c r="U62" s="10"/>
+      <c r="V62" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="W62" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="X62" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="Y62" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z62" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA62" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="J63" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="K63" s="2">
+        <v>10.8</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="N63" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="O63" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P63" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R63" s="10"/>
+      <c r="S63" s="10"/>
+      <c r="T63" s="10"/>
+      <c r="U63" s="10"/>
+      <c r="V63" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="Y63" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z63" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA63" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="J64" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="K64" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="N64" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O64" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P64" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10"/>
+      <c r="U64" s="10"/>
+      <c r="V64" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="Y64" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z64" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA64" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="J65" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="K65" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="M65" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="N65" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O65" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P65" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
+      <c r="V65" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y65" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z65" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA65" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="J66" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="K66" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="N66" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="O66" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P66" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
+      <c r="V66" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="W66" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="X66" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="Y66" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z66" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA66" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="J67" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="K67" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L67" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="N67" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O67" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P67" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q67" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="10"/>
+      <c r="V67" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="W67" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="X67" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="Y67" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z67" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA67" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="J68" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="K68" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L68" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="N68" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O68" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P68" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
+      <c r="U68" s="10"/>
+      <c r="V68" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="W68" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="X68" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="Y68" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z68" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA68" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="J69" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="K69" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="N69" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="O69" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P69" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q69" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="10"/>
+      <c r="V69" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="W69" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="X69" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="Y69" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z69" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA69" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K70" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="N70" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O70" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P70" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q70" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
+      <c r="U70" s="10"/>
+      <c r="V70" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="W70" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="X70" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="Y70" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="Z70" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA70" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K71" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="M71" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="N71" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O71" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P71" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R71" s="10"/>
+      <c r="S71" s="10"/>
+      <c r="T71" s="10"/>
+      <c r="U71" s="10"/>
+      <c r="V71" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y71" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z71" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="AA71" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>682</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K72" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="N72" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O72" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P72" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q72" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10"/>
+      <c r="U72" s="10"/>
+      <c r="V72" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="Y72" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="Z72" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="AA72" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>690</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K73" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="M73" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="N73" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O73" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P73" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q73" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R73" s="10"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="10"/>
+      <c r="U73" s="10"/>
+      <c r="V73" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="Y73" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="Z73" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="AA73" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K74" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="N74" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O74" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="P74" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
+      <c r="U74" s="10"/>
+      <c r="V74" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="W74" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="X74" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="Y74" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z74" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="AA74" s="4" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K75" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="N75" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="O75" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P75" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
+      <c r="U75" s="10"/>
+      <c r="V75" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="W75" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="X75" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="Y75" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z75" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="AA75" s="4" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K76" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="N76" s="10"/>
+      <c r="O76" s="10"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="10"/>
+      <c r="R76" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="S76" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="T76" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="U76" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="V76" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="W76" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="X76" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="Y76" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z76" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA76" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="V77" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4231,7 +8127,85 @@
     <hyperlink r:id="rId70" ref="D36"/>
     <hyperlink r:id="rId71" ref="C37"/>
     <hyperlink r:id="rId72" ref="D37"/>
+    <hyperlink r:id="rId73" ref="C38"/>
+    <hyperlink r:id="rId74" ref="D38"/>
+    <hyperlink r:id="rId75" ref="C39"/>
+    <hyperlink r:id="rId76" ref="D39"/>
+    <hyperlink r:id="rId77" ref="C40"/>
+    <hyperlink r:id="rId78" ref="D40"/>
+    <hyperlink r:id="rId79" ref="C41"/>
+    <hyperlink r:id="rId80" ref="D41"/>
+    <hyperlink r:id="rId81" ref="C42"/>
+    <hyperlink r:id="rId82" ref="D42"/>
+    <hyperlink r:id="rId83" ref="C43"/>
+    <hyperlink r:id="rId84" ref="D43"/>
+    <hyperlink r:id="rId85" ref="C44"/>
+    <hyperlink r:id="rId86" ref="D44"/>
+    <hyperlink r:id="rId87" ref="C45"/>
+    <hyperlink r:id="rId88" ref="D45"/>
+    <hyperlink r:id="rId89" ref="C46"/>
+    <hyperlink r:id="rId90" ref="D46"/>
+    <hyperlink r:id="rId91" ref="C47"/>
+    <hyperlink r:id="rId92" ref="D47"/>
+    <hyperlink r:id="rId93" ref="C48"/>
+    <hyperlink r:id="rId94" ref="D48"/>
+    <hyperlink r:id="rId95" ref="C49"/>
+    <hyperlink r:id="rId96" ref="D49"/>
+    <hyperlink r:id="rId97" ref="C50"/>
+    <hyperlink r:id="rId98" ref="D50"/>
+    <hyperlink r:id="rId99" ref="C51"/>
+    <hyperlink r:id="rId100" ref="D51"/>
+    <hyperlink r:id="rId101" ref="C52"/>
+    <hyperlink r:id="rId102" ref="D52"/>
+    <hyperlink r:id="rId103" ref="C53"/>
+    <hyperlink r:id="rId104" ref="D53"/>
+    <hyperlink r:id="rId105" ref="C54"/>
+    <hyperlink r:id="rId106" ref="D54"/>
+    <hyperlink r:id="rId107" ref="C55"/>
+    <hyperlink r:id="rId108" ref="D55"/>
+    <hyperlink r:id="rId109" ref="C56"/>
+    <hyperlink r:id="rId110" ref="D56"/>
+    <hyperlink r:id="rId111" ref="C57"/>
+    <hyperlink r:id="rId112" ref="D57"/>
+    <hyperlink r:id="rId113" ref="C58"/>
+    <hyperlink r:id="rId114" ref="D58"/>
+    <hyperlink r:id="rId115" ref="C59"/>
+    <hyperlink r:id="rId116" ref="D59"/>
+    <hyperlink r:id="rId117" ref="C60"/>
+    <hyperlink r:id="rId118" ref="D60"/>
+    <hyperlink r:id="rId119" ref="C61"/>
+    <hyperlink r:id="rId120" ref="D61"/>
+    <hyperlink r:id="rId121" ref="C62"/>
+    <hyperlink r:id="rId122" ref="D62"/>
+    <hyperlink r:id="rId123" ref="C63"/>
+    <hyperlink r:id="rId124" ref="D63"/>
+    <hyperlink r:id="rId125" ref="C64"/>
+    <hyperlink r:id="rId126" ref="D64"/>
+    <hyperlink r:id="rId127" ref="C65"/>
+    <hyperlink r:id="rId128" ref="D65"/>
+    <hyperlink r:id="rId129" ref="C66"/>
+    <hyperlink r:id="rId130" ref="D66"/>
+    <hyperlink r:id="rId131" ref="C67"/>
+    <hyperlink r:id="rId132" ref="D67"/>
+    <hyperlink r:id="rId133" ref="C68"/>
+    <hyperlink r:id="rId134" ref="D68"/>
+    <hyperlink r:id="rId135" ref="C69"/>
+    <hyperlink r:id="rId136" ref="D69"/>
+    <hyperlink r:id="rId137" ref="C70"/>
+    <hyperlink r:id="rId138" ref="D70"/>
+    <hyperlink r:id="rId139" ref="C71"/>
+    <hyperlink r:id="rId140" ref="D71"/>
+    <hyperlink r:id="rId141" ref="C72"/>
+    <hyperlink r:id="rId142" ref="D72"/>
+    <hyperlink r:id="rId143" ref="C73"/>
+    <hyperlink r:id="rId144" ref="D73"/>
+    <hyperlink r:id="rId145" ref="C74"/>
+    <hyperlink r:id="rId146" ref="D74"/>
+    <hyperlink r:id="rId147" ref="C75"/>
+    <hyperlink r:id="rId148" ref="D75"/>
+    <hyperlink r:id="rId149" ref="C76"/>
+    <hyperlink r:id="rId150" ref="D76"/>
   </hyperlinks>
-  <drawing r:id="rId73"/>
+  <drawing r:id="rId151"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Converted raw sleeve images to PNG. Applied machine learning to get top 3 recommendations, word cloud, and most important feature results.
</commit_message>
<xml_diff>
--- a/RawData.xlsx
+++ b/RawData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="731">
   <si>
     <t>ID</t>
   </si>
@@ -1890,6 +1890,9 @@
   </si>
   <si>
     <t>https://www.nespresso.com/ecom/medias/sys_master/public/14446104870942/voltessio-XL.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/vl/voltesso_XL.png?impolicy=medium&amp;imwidth=824&amp;imdensity=1</t>
   </si>
   <si>
     <t>Light &amp; Sweet</t>
@@ -7250,7 +7253,7 @@
         <v>625</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>619</v>
+        <v>626</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>377</v>
@@ -7265,7 +7268,7 @@
         <v>115</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J66" s="2">
         <v>4.0</v>
@@ -7277,7 +7280,7 @@
         <v>96</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="N66" s="2">
         <v>2.0</v>
@@ -7296,13 +7299,13 @@
       <c r="T66" s="10"/>
       <c r="U66" s="10"/>
       <c r="V66" s="4" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="W66" s="4" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="X66" s="4" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="Y66" s="4" t="s">
         <v>41</v>
@@ -7311,21 +7314,21 @@
         <v>507</v>
       </c>
       <c r="AA66" s="4" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>377</v>
@@ -7337,10 +7340,10 @@
         <v>570</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="J67" s="2">
         <v>11.0</v>
@@ -7352,7 +7355,7 @@
         <v>96</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="N67" s="2">
         <v>1.0</v>
@@ -7371,13 +7374,13 @@
       <c r="T67" s="10"/>
       <c r="U67" s="10"/>
       <c r="V67" s="4" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="W67" s="4" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="X67" s="4" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="Y67" s="4" t="s">
         <v>41</v>
@@ -7386,21 +7389,21 @@
         <v>507</v>
       </c>
       <c r="AA67" s="4" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>377</v>
@@ -7412,10 +7415,10 @@
         <v>570</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J68" s="2">
         <v>8.0</v>
@@ -7427,7 +7430,7 @@
         <v>96</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="N68" s="2">
         <v>1.0</v>
@@ -7446,13 +7449,13 @@
       <c r="T68" s="10"/>
       <c r="U68" s="10"/>
       <c r="V68" s="4" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="W68" s="4" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="X68" s="4" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="Y68" s="4" t="s">
         <v>41</v>
@@ -7461,21 +7464,21 @@
         <v>507</v>
       </c>
       <c r="AA68" s="4" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>377</v>
@@ -7487,10 +7490,10 @@
         <v>570</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="J69" s="2">
         <v>5.0</v>
@@ -7502,7 +7505,7 @@
         <v>425</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="N69" s="2">
         <v>2.0</v>
@@ -7521,13 +7524,13 @@
       <c r="T69" s="10"/>
       <c r="U69" s="10"/>
       <c r="V69" s="4" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="W69" s="4" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="X69" s="4" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="Y69" s="4" t="s">
         <v>41</v>
@@ -7541,16 +7544,16 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>377</v>
@@ -7562,7 +7565,7 @@
         <v>272</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>292</v>
@@ -7574,10 +7577,10 @@
         <v>12.6</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="N70" s="2">
         <v>1.0</v>
@@ -7596,16 +7599,16 @@
       <c r="T70" s="10"/>
       <c r="U70" s="10"/>
       <c r="V70" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="W70" s="4" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="X70" s="4" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="Y70" s="4" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="Z70" s="4" t="s">
         <v>507</v>
@@ -7616,16 +7619,16 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>377</v>
@@ -7637,7 +7640,7 @@
         <v>272</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>301</v>
@@ -7649,10 +7652,10 @@
         <v>12.6</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="N71" s="2">
         <v>1.0</v>
@@ -7671,7 +7674,7 @@
       <c r="T71" s="10"/>
       <c r="U71" s="10"/>
       <c r="V71" s="4" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Y71" s="4" t="s">
         <v>305</v>
@@ -7685,16 +7688,16 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>377</v>
@@ -7706,7 +7709,7 @@
         <v>272</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>284</v>
@@ -7718,10 +7721,10 @@
         <v>12.6</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="N72" s="2">
         <v>1.0</v>
@@ -7740,13 +7743,13 @@
       <c r="T72" s="10"/>
       <c r="U72" s="10"/>
       <c r="V72" s="4" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="Y72" s="4" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Z72" s="4" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="AA72" s="4" t="s">
         <v>394</v>
@@ -7754,16 +7757,16 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>377</v>
@@ -7775,10 +7778,10 @@
         <v>272</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>275</v>
@@ -7787,10 +7790,10 @@
         <v>12.6</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="N73" s="2">
         <v>1.0</v>
@@ -7809,13 +7812,13 @@
       <c r="T73" s="10"/>
       <c r="U73" s="10"/>
       <c r="V73" s="4" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="Y73" s="4" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="Z73" s="4" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="AA73" s="4" t="s">
         <v>394</v>
@@ -7823,16 +7826,16 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>377</v>
@@ -7844,10 +7847,10 @@
         <v>272</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>275</v>
@@ -7856,10 +7859,10 @@
         <v>9.9</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="N74" s="2">
         <v>1.0</v>
@@ -7878,36 +7881,36 @@
       <c r="T74" s="10"/>
       <c r="U74" s="10"/>
       <c r="V74" s="4" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="W74" s="4" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="X74" s="4" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="Y74" s="4" t="s">
         <v>41</v>
       </c>
       <c r="Z74" s="4" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AA74" s="4" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>377</v>
@@ -7919,10 +7922,10 @@
         <v>272</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>275</v>
@@ -7934,7 +7937,7 @@
         <v>257</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="N75" s="13">
         <v>0.0</v>
@@ -7953,36 +7956,36 @@
       <c r="T75" s="10"/>
       <c r="U75" s="10"/>
       <c r="V75" s="4" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="W75" s="4" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="X75" s="4" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="Y75" s="4" t="s">
         <v>41</v>
       </c>
       <c r="Z75" s="4" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AA75" s="4" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>377</v>
@@ -7994,7 +7997,7 @@
         <v>272</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>521</v>
@@ -8006,10 +8009,10 @@
         <v>12.6</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="N76" s="10"/>
       <c r="O76" s="10"/>
@@ -8028,13 +8031,13 @@
         <v>3.0</v>
       </c>
       <c r="V76" s="4" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="W76" s="4" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="X76" s="4" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="Y76" s="4" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added current ice coffee, adjusted functions accordingly. Changed naming convention for guides.
</commit_message>
<xml_diff>
--- a/RawData.xlsx
+++ b/RawData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="750">
   <si>
     <t>ID</t>
   </si>
@@ -2205,6 +2205,63 @@
   </si>
   <si>
     <t>One part of the blend gets a long and dark roast, while the second part is roasted a little faster and to a slightly lighter degree.</t>
+  </si>
+  <si>
+    <t>VL40</t>
+  </si>
+  <si>
+    <t>Ice Forte</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15389833166878/C-0920-ice-forte-XL-responsive-plp-image.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/next-components/assets/summer-22/sku-main-info/vl-coffee-sleeves_ice-forte_1-1_d_@2x.png</t>
+  </si>
+  <si>
+    <t>230 ml (Coffee) &amp; Iced Recipe</t>
+  </si>
+  <si>
+    <t>For intense recipes with ice</t>
+  </si>
+  <si>
+    <t>Barista Creations Ice Forte carries that distinct roasted character that’ll truly awaken your senses. Cereal, woody and peppery notes lace through the cup to deliver a rich iced coffee experience.</t>
+  </si>
+  <si>
+    <t>Why we love it: Enjoy the intense taste of Barista Creations ICE FORTE in a refreshing coffee over ice. South American Arabicas mix with the Indonesian and Ethiopian Arabicas to offer an impactful aromatic experience. Dark roasted and ground specifically for a delicious coffee over ice. Best served as: 1 coffee capsule (230 ml) over a cup full of ice cubes (230 g). To prolong the pleasure, top it up with cold water or cold milk (180 ml).</t>
+  </si>
+  <si>
+    <t>This 100% Arabica blend is made mostly with a combination of Colombian, Indonesian and Ethiopian beans.</t>
+  </si>
+  <si>
+    <t>Part of this blend gets a medium roast to keep the flavour complexity intact. The other part gets a longer and darker roast to delivers intensity and a bold body.</t>
+  </si>
+  <si>
+    <t>VL41</t>
+  </si>
+  <si>
+    <t>Ice Leggero</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15390013358110/C-0919-Responsive-plp-image.png?impolicy=small&amp;imwidth=284&amp;imdensity=1</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/next-components/assets/summer-22/sku-main-info/vl-coffee-sleeves_ice-leggero_16_9_m_@2x.png</t>
+  </si>
+  <si>
+    <t>For mild recipes with ice</t>
+  </si>
+  <si>
+    <t>Chill out with the light and thirst-quenching fruitiness of this refreshing iced coffee experience, paired with a rounded cereal note.</t>
+  </si>
+  <si>
+    <t>Why we love it: Enjoy the delicate fruity and cereal notes of Barista Creations Ice Leggero. The elegant flavours of the Ethiopian Arabica in this blend refresh you like the most gentle summer breeze when you pour it over ice. We roast it lightly and grind it specifically to deliver that cool, delicate taste to your palate. Best served as: 1 coffee capsule (80 ml) over a cup full of ice cubes (180 g). To prolong the pleasure, top it up with cold water or cold milk (180 ml).</t>
+  </si>
+  <si>
+    <t>This 100% Arabica blend gets its coffee mostly from Ethiopia and Indonesia.</t>
+  </si>
+  <si>
+    <t>The first part of this blend gets a light and short roast to enhance the floral notes typical of Ethiopian Arabica. The second gets a medium roast to bring balance and roundness to the cup.</t>
   </si>
 </sst>
 </file>
@@ -8050,11 +8107,138 @@
       </c>
     </row>
     <row r="77">
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="V77" s="4"/>
+      <c r="A77" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K77" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="N77" s="10"/>
+      <c r="O77" s="10"/>
+      <c r="P77" s="10"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="10"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="10"/>
+      <c r="U77" s="10"/>
+      <c r="V77" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="W77" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="X77" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="Y77" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z77" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA77" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>743</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K78" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="N78" s="10"/>
+      <c r="O78" s="10"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="10"/>
+      <c r="R78" s="10"/>
+      <c r="S78" s="10"/>
+      <c r="T78" s="10"/>
+      <c r="U78" s="10"/>
+      <c r="V78" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="W78" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="X78" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="Y78" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="Z78" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA78" s="4" t="s">
+        <v>643</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8208,7 +8392,11 @@
     <hyperlink r:id="rId148" ref="D75"/>
     <hyperlink r:id="rId149" ref="C76"/>
     <hyperlink r:id="rId150" ref="D76"/>
+    <hyperlink r:id="rId151" ref="C77"/>
+    <hyperlink r:id="rId152" ref="D77"/>
+    <hyperlink r:id="rId153" ref="C78"/>
+    <hyperlink r:id="rId154" ref="D78"/>
   </hyperlinks>
-  <drawing r:id="rId151"/>
+  <drawing r:id="rId155"/>
 </worksheet>
 </file>
</xml_diff>